<commit_message>
All present value calculations via python code
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_its.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_its.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="645" windowWidth="13680" windowHeight="11250" tabRatio="847"/>
+    <workbookView xWindow="480" yWindow="645" windowWidth="13680" windowHeight="11250" tabRatio="847" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -335,9 +335,6 @@
     <t>IRR</t>
   </si>
   <si>
-    <t>Approx OPEX per year per subscriber</t>
-  </si>
-  <si>
     <t>PS+ONT+DSLAM</t>
   </si>
   <si>
@@ -537,6 +534,9 @@
   </si>
   <si>
     <t>FTTB_Hybridpon_120</t>
+  </si>
+  <si>
+    <t>Approx OPEX per year</t>
   </si>
 </sst>
 </file>
@@ -1257,11 +1257,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="188035584"/>
-        <c:axId val="223728704"/>
+        <c:axId val="63445504"/>
+        <c:axId val="70636608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="188035584"/>
+        <c:axId val="63445504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1289,7 +1289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223728704"/>
+        <c:crossAx val="70636608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1297,7 +1297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223728704"/>
+        <c:axId val="70636608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,7 +1327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188035584"/>
+        <c:crossAx val="63445504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1379,6 +1379,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1397,7 +1398,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Approx OPEX per year per subscriber</c:v>
+                  <c:v>Approx OPEX per year</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1514,11 +1515,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="188036608"/>
-        <c:axId val="223730432"/>
+        <c:axId val="63714816"/>
+        <c:axId val="63537152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="188036608"/>
+        <c:axId val="63714816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,7 +1528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223730432"/>
+        <c:crossAx val="63537152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1535,7 +1536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223730432"/>
+        <c:axId val="63537152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,13 +1559,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188036608"/>
+        <c:crossAx val="63714816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2091,11 +2093,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="220953088"/>
-        <c:axId val="228098624"/>
+        <c:axId val="64286720"/>
+        <c:axId val="70638912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="220953088"/>
+        <c:axId val="64286720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2105,7 +2107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228098624"/>
+        <c:crossAx val="70638912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2113,7 +2115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228098624"/>
+        <c:axId val="70638912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2124,7 +2126,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220953088"/>
+        <c:crossAx val="64286720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2539,7 +2541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -2568,10 +2570,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -2592,7 +2594,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>5</v>
@@ -2631,7 +2633,7 @@
         <v>19</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X1" s="9" t="s">
         <v>20</v>
@@ -2679,7 +2681,7 @@
     </row>
     <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="7">
         <v>342</v>
@@ -2698,7 +2700,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" s="7">
         <f>0.64</f>
@@ -2762,7 +2764,7 @@
     </row>
     <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="7">
         <v>342</v>
@@ -2844,7 +2846,7 @@
     </row>
     <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="7">
         <v>342</v>
@@ -2922,7 +2924,7 @@
     </row>
     <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="7">
         <v>2049</v>
@@ -3004,7 +3006,7 @@
     </row>
     <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="7">
         <v>2049</v>
@@ -3086,7 +3088,7 @@
     </row>
     <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="7">
         <v>342</v>
@@ -3104,7 +3106,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H8" s="7">
         <v>1.3</v>
@@ -3166,7 +3168,7 @@
     </row>
     <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="7">
         <v>342</v>
@@ -3246,7 +3248,7 @@
     </row>
     <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="7">
         <v>342</v>
@@ -3325,7 +3327,7 @@
     </row>
     <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="7">
         <v>342</v>
@@ -3344,7 +3346,7 @@
         <v>21</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="7">
         <v>0.54</v>
@@ -3406,7 +3408,7 @@
     </row>
     <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="7">
         <v>342</v>
@@ -3486,7 +3488,7 @@
     </row>
     <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="7">
         <v>2049</v>
@@ -3567,7 +3569,7 @@
     </row>
     <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="7">
         <v>342</v>
@@ -3585,7 +3587,7 @@
         <v>21</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="7">
         <v>0.54</v>
@@ -3647,7 +3649,7 @@
     </row>
     <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="7">
         <v>342</v>
@@ -3734,7 +3736,7 @@
     </row>
     <row r="42" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R42" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
@@ -3743,17 +3745,17 @@
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
       <c r="Y42" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S44">
         <f>0.02/1000</f>
@@ -3768,23 +3770,23 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="Y44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S45" t="s">
+        <v>57</v>
+      </c>
+      <c r="T45" t="s">
         <v>58</v>
       </c>
-      <c r="T45" t="s">
+      <c r="W45" t="s">
         <v>59</v>
-      </c>
-      <c r="W45" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="46" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S46">
         <v>1.1200000000000001</v>
@@ -3796,7 +3798,7 @@
         <v>0.73</v>
       </c>
       <c r="Y46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3830,13 +3832,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -3851,13 +3853,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -3872,13 +3874,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -5275,13 +5277,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -5296,13 +5298,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -5317,13 +5319,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -6723,13 +6725,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -6744,13 +6746,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -6765,13 +6767,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -8168,13 +8170,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -8189,13 +8191,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -8210,13 +8212,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -9613,13 +9615,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -9634,13 +9636,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -9655,13 +9657,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -11058,13 +11060,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -11079,13 +11081,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -11100,13 +11102,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -12503,13 +12505,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -12524,13 +12526,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -12545,13 +12547,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -13948,13 +13950,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -13969,13 +13971,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -13990,13 +13992,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -15404,43 +15406,43 @@
         <v>23</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -15505,7 +15507,7 @@
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -15556,7 +15558,7 @@
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -15605,7 +15607,7 @@
     </row>
     <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -15654,7 +15656,7 @@
     </row>
     <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -15701,7 +15703,7 @@
     </row>
     <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -15748,7 +15750,7 @@
     </row>
     <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -15797,7 +15799,7 @@
     </row>
     <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -15845,7 +15847,7 @@
     </row>
     <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -15893,7 +15895,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -15944,7 +15946,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -15993,7 +15995,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -16040,7 +16042,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -16089,7 +16091,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -16161,7 +16163,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16176,7 +16178,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -16189,7 +16191,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="12">
         <f>0.1*(CAPEX!U3+CAPEX!V3)+0.01*(CAPEX!S3+CAPEX!T3)</f>
@@ -16198,7 +16200,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="12">
         <f>0.1*(CAPEX!U4+CAPEX!V4)+0.01*(CAPEX!S4+CAPEX!T4)</f>
@@ -16207,7 +16209,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="12">
         <f>0.1*(CAPEX!U5+CAPEX!V5)+0.01*(CAPEX!S5+CAPEX!T5)</f>
@@ -16216,7 +16218,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="12">
         <f>0.1*(CAPEX!U6+CAPEX!V6)+0.01*(CAPEX!S6+CAPEX!T6)</f>
@@ -16225,7 +16227,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="12">
         <f>0.1*(CAPEX!U7+CAPEX!V7)+0.01*(CAPEX!S7+CAPEX!T7)</f>
@@ -16234,7 +16236,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="12">
         <f>0.1*(CAPEX!U8+CAPEX!V8)+0.01*(CAPEX!S8+CAPEX!T8)</f>
@@ -16243,7 +16245,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="12">
         <f>0.1*(CAPEX!U9+CAPEX!V9)+0.01*(CAPEX!S9+CAPEX!T9)</f>
@@ -16252,7 +16254,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="12">
         <f>0.1*(CAPEX!U10+CAPEX!V10)+0.01*(CAPEX!S10+CAPEX!T10)</f>
@@ -16261,7 +16263,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="12">
         <f>0.1*(CAPEX!U11+CAPEX!V11)+0.01*(CAPEX!S11+CAPEX!T11)</f>
@@ -16270,7 +16272,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="12">
         <f>0.1*(CAPEX!U12+CAPEX!V12)+0.01*(CAPEX!S12+CAPEX!T12)</f>
@@ -16279,7 +16281,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="12">
         <f>0.1*(CAPEX!U13+CAPEX!V13)+0.01*(CAPEX!S13+CAPEX!T13)</f>
@@ -16288,7 +16290,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="12">
         <f>0.1*(CAPEX!U14+CAPEX!V14)+0.01*(CAPEX!S14+CAPEX!T14)</f>
@@ -16297,7 +16299,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="12">
         <f>0.1*(CAPEX!U15+CAPEX!V15)+0.01*(CAPEX!S15+CAPEX!T15)</f>
@@ -16314,7 +16316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH74"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5:H18"/>
     </sheetView>
   </sheetViews>
@@ -16362,13 +16364,13 @@
         <v>29</v>
       </c>
       <c r="R1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="U1" s="10" t="s">
         <v>30</v>
@@ -16383,13 +16385,13 @@
         <v>33</v>
       </c>
       <c r="Y1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="AB1" s="10" t="s">
         <v>34</v>
@@ -16404,13 +16406,13 @@
         <v>37</v>
       </c>
       <c r="AF1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="AH1" s="10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -16430,7 +16432,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="M2" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N2" s="7">
         <v>2018</v>
@@ -16532,7 +16534,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="M3" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N3" s="7">
         <v>2019</v>
@@ -16634,16 +16636,16 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="H4" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>85</v>
-      </c>
       <c r="J4" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N4" s="7">
         <v>2020</v>
@@ -16755,7 +16757,7 @@
         <v>3.6</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N5" s="7">
         <v>2021</v>
@@ -16857,7 +16859,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="H6" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I6" s="10">
         <f>30*12/50</f>
@@ -16867,7 +16869,7 @@
         <v>12</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" s="7">
         <v>2022</v>
@@ -16969,7 +16971,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="H7" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="10">
         <f>40*12/50</f>
@@ -16979,7 +16981,7 @@
         <v>24</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N7" s="7">
         <v>2023</v>
@@ -17081,7 +17083,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="H8" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="10">
         <f>40*12/50</f>
@@ -17091,7 +17093,7 @@
         <v>24</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N8" s="7">
         <v>2024</v>
@@ -17193,7 +17195,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="H9" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="10">
         <v>12</v>
@@ -17202,7 +17204,7 @@
         <v>36</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N9" s="7">
         <v>2025</v>
@@ -17304,7 +17306,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="H10" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="10">
         <v>12</v>
@@ -17313,7 +17315,7 @@
         <v>36</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N10" s="7">
         <v>2026</v>
@@ -17415,7 +17417,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="H11" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I11" s="10">
         <v>12</v>
@@ -17424,7 +17426,7 @@
         <v>36</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N11" s="7">
         <v>2027</v>
@@ -17526,7 +17528,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="H12" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12" s="10">
         <f>50*12/50</f>
@@ -17536,7 +17538,7 @@
         <v>36</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N12" s="7">
         <v>2028</v>
@@ -17638,7 +17640,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="H13" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I13" s="10">
         <v>12</v>
@@ -17647,7 +17649,7 @@
         <v>36</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N13" s="7">
         <v>2029</v>
@@ -17749,7 +17751,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="H14" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="10">
         <v>7.2</v>
@@ -17758,7 +17760,7 @@
         <v>12</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N14" s="7">
         <v>2030</v>
@@ -17860,7 +17862,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="H15" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="10">
         <v>9.6</v>
@@ -17869,7 +17871,7 @@
         <v>24</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N15" s="7">
         <v>2031</v>
@@ -17971,7 +17973,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="H16" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" s="10">
         <v>12</v>
@@ -17980,7 +17982,7 @@
         <v>36</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N16" s="7">
         <v>2032</v>
@@ -18082,7 +18084,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="H17" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I17" s="10">
         <v>12</v>
@@ -18091,7 +18093,7 @@
         <v>36</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N17" s="7">
         <v>2033</v>
@@ -18193,7 +18195,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="H18" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18" s="10">
         <v>12</v>
@@ -18202,7 +18204,7 @@
         <v>36</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N18" s="7">
         <v>2034</v>
@@ -18304,7 +18306,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="M19" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N19" s="7">
         <v>2035</v>
@@ -18406,7 +18408,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="M20" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N20" s="7">
         <v>2036</v>
@@ -18508,7 +18510,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="M21" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N21" s="7">
         <v>2037</v>
@@ -18610,7 +18612,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="M22" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N22" s="7">
         <v>2038</v>
@@ -18709,10 +18711,10 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -18729,13 +18731,13 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" t="s">
         <v>42</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>43</v>
-      </c>
-      <c r="G28" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
@@ -18767,10 +18769,10 @@
         <v>80</v>
       </c>
       <c r="J29" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" t="s">
         <v>80</v>
-      </c>
-      <c r="K29" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
@@ -19375,7 +19377,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -19392,13 +19394,13 @@
         <v>27</v>
       </c>
       <c r="E53" t="s">
+        <v>41</v>
+      </c>
+      <c r="F53" t="s">
         <v>42</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>43</v>
-      </c>
-      <c r="G53" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -20043,13 +20045,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -20064,13 +20066,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -20085,13 +20087,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -21489,13 +21491,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -21510,13 +21512,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -21531,13 +21533,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -22934,13 +22936,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -22955,13 +22957,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -22976,13 +22978,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -24379,13 +24381,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -24400,13 +24402,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -24421,13 +24423,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -25824,13 +25826,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -25845,13 +25847,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -25866,13 +25868,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -27269,13 +27271,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -27290,13 +27292,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -27311,13 +27313,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
error in input data
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_its.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_its.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="705" windowWidth="13680" windowHeight="11190" tabRatio="847" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="705" windowWidth="13680" windowHeight="11190" tabRatio="847" firstSheet="7" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="FTTB_Hybridpon_100" sheetId="19" r:id="rId17"/>
     <sheet name="MIG_MATRIX" sheetId="11" r:id="rId18"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId19"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -796,6 +799,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1127,7 +1131,7 @@
                   <c:v>12818.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11216.333333333334</c:v>
+                  <c:v>5866.833333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4000</c:v>
@@ -1139,7 +1143,7 @@
                   <c:v>14160</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27600</c:v>
+                  <c:v>14800</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>14160</c:v>
@@ -1279,11 +1283,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="162805248"/>
-        <c:axId val="161329664"/>
+        <c:axId val="62907904"/>
+        <c:axId val="133455168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="162805248"/>
+        <c:axId val="62907904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,13 +1309,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161329664"/>
+        <c:crossAx val="133455168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1319,7 +1324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161329664"/>
+        <c:axId val="133455168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,19 +1347,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162805248"/>
+        <c:crossAx val="62907904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1370,6 +1377,613 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Capital Expenditure of various technologies in business scenario</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]CAPEX!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duct Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]CAPEX!$A$3:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>FTTC_GPON_25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTTB_XGPON_50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTTB_UDWDM_50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTTH_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTTH_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FTTC_GPON_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FTTB_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FTTB_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FTTC_Hybridpon_25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FTTB_Hybridpon_50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FTTH_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>FTTC_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>FTTB_Hybridpon_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]CAPEX!$S$3:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>146337.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146337.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78872.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78872.09</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>146337.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>146337.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146337.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78872.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>114876.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>115530.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>115530.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>114876.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>115530.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]CAPEX!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fiber Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]CAPEX!$A$3:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>FTTC_GPON_25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTTB_XGPON_50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTTB_UDWDM_50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTTH_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTTH_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FTTC_GPON_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FTTB_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FTTB_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FTTC_Hybridpon_25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FTTB_Hybridpon_50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FTTH_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>FTTC_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>FTTB_Hybridpon_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]CAPEX!$T$3:$T$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>18.840229999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.814590000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.612120000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.612120000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.814590000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.840229999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.814590000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.612120000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.59423</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.21167</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.08727</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.59423</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.21167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]CAPEX!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CO cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]CAPEX!$A$3:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>FTTC_GPON_25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTTB_XGPON_50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTTB_UDWDM_50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTTH_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTTH_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FTTC_GPON_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FTTB_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FTTB_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FTTC_Hybridpon_25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FTTB_Hybridpon_50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FTTH_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>FTTC_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>FTTB_Hybridpon_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]CAPEX!$U$3:$U$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3056.8888888888887</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6405.333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5299.166666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5866.833333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12618.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6426.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12818.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5866.833333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]CAPEX!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RN Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]CAPEX!$A$3:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>FTTC_GPON_25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTTB_XGPON_50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTTB_UDWDM_50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTTH_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTTH_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FTTC_GPON_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FTTB_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FTTB_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FTTC_Hybridpon_25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FTTB_Hybridpon_50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FTTH_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>FTTC_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>FTTB_Hybridpon_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]CAPEX!$V$3:$V$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>158553.60000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63750.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60860</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133338.59999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>129280.20000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>195086.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61989.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63060</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96145</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55966.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>168466.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105356</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66966.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="62909952"/>
+        <c:axId val="133588096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="62909952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Technology</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133588096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="133588096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Cost in C.U.</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62909952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -1481,7 +2095,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>36062.342937580564</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19283.042118970367</c:v>
@@ -1540,11 +2154,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="164097024"/>
-        <c:axId val="161331968"/>
+        <c:axId val="163129856"/>
+        <c:axId val="133590400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164097024"/>
+        <c:axId val="163129856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +2168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161331968"/>
+        <c:crossAx val="133590400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1562,7 +2176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161331968"/>
+        <c:axId val="133590400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,7 +2206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164097024"/>
+        <c:crossAx val="163129856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1609,7 +2223,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -2134,11 +2748,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101306880"/>
-        <c:axId val="163700032"/>
+        <c:axId val="163478016"/>
+        <c:axId val="133592128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101306880"/>
+        <c:axId val="163478016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2148,7 +2762,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163700032"/>
+        <c:crossAx val="133592128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2156,7 +2770,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163700032"/>
+        <c:axId val="133592128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,7 +2781,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101306880"/>
+        <c:crossAx val="163478016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2221,6 +2835,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1674284</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2309,6 +2961,328 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="CAPEX"/>
+      <sheetName val="OPEX"/>
+      <sheetName val="Revenue"/>
+      <sheetName val="ADSL"/>
+      <sheetName val="FTTC_GPON_25"/>
+      <sheetName val="FTTB_XGPON_50"/>
+      <sheetName val="FTTB_UDWDM_50"/>
+      <sheetName val="FTTH_UDWDM_100"/>
+      <sheetName val="FTTH_XGPON_100"/>
+      <sheetName val="FTTC_GPON_100"/>
+      <sheetName val="FTTB_XGPON_100"/>
+      <sheetName val="FTTB_UDWDM_100"/>
+      <sheetName val="FTTC_Hybridpon_25"/>
+      <sheetName val="FTTB_Hybridpon_50"/>
+      <sheetName val="FTTH_Hybridpon_100"/>
+      <sheetName val="FTTC_Hybridpon_100"/>
+      <sheetName val="FTTB_Hybridpon_100"/>
+      <sheetName val="MIG_MATRIX"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="S1" t="str">
+            <v>Duct Cost</v>
+          </cell>
+          <cell r="T1" t="str">
+            <v>Fiber Cost</v>
+          </cell>
+          <cell r="U1" t="str">
+            <v>CO cost</v>
+          </cell>
+          <cell r="V1" t="str">
+            <v>RN Cost</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>FTTC_GPON_25</v>
+          </cell>
+          <cell r="S3">
+            <v>146337.9</v>
+          </cell>
+          <cell r="T3">
+            <v>18.840229999999998</v>
+          </cell>
+          <cell r="U3">
+            <v>3056.8888888888887</v>
+          </cell>
+          <cell r="V3">
+            <v>158553.60000000001</v>
+          </cell>
+          <cell r="X3">
+            <v>307967.22911888885</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>FTTB_XGPON_50</v>
+          </cell>
+          <cell r="S4">
+            <v>146337.9</v>
+          </cell>
+          <cell r="T4">
+            <v>12.814590000000001</v>
+          </cell>
+          <cell r="U4">
+            <v>6405.333333333333</v>
+          </cell>
+          <cell r="V4">
+            <v>63750.8</v>
+          </cell>
+          <cell r="X4">
+            <v>216506.84792333335</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>FTTB_UDWDM_50</v>
+          </cell>
+          <cell r="S5">
+            <v>78872.09</v>
+          </cell>
+          <cell r="T5">
+            <v>14.612120000000001</v>
+          </cell>
+          <cell r="U5">
+            <v>5299.166666666667</v>
+          </cell>
+          <cell r="V5">
+            <v>60860</v>
+          </cell>
+          <cell r="X5">
+            <v>145045.86878666666</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>FTTH_UDWDM_100</v>
+          </cell>
+          <cell r="S6">
+            <v>78872.09</v>
+          </cell>
+          <cell r="T6">
+            <v>14.612120000000001</v>
+          </cell>
+          <cell r="U6">
+            <v>5866.833333333333</v>
+          </cell>
+          <cell r="V6">
+            <v>133338.59999999998</v>
+          </cell>
+          <cell r="X6">
+            <v>218092.13545333332</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>FTTH_XGPON_100</v>
+          </cell>
+          <cell r="S7">
+            <v>146337.9</v>
+          </cell>
+          <cell r="T7">
+            <v>12.814590000000001</v>
+          </cell>
+          <cell r="U7">
+            <v>12618.666666666666</v>
+          </cell>
+          <cell r="V7">
+            <v>129280.20000000001</v>
+          </cell>
+          <cell r="X7">
+            <v>288249.58125666669</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>FTTC_GPON_100</v>
+          </cell>
+          <cell r="S8">
+            <v>146337.9</v>
+          </cell>
+          <cell r="T8">
+            <v>18.840229999999998</v>
+          </cell>
+          <cell r="U8">
+            <v>6426.666666666667</v>
+          </cell>
+          <cell r="V8">
+            <v>195086.4</v>
+          </cell>
+          <cell r="X8">
+            <v>347869.80689666665</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>FTTB_XGPON_100</v>
+          </cell>
+          <cell r="S9">
+            <v>146337.9</v>
+          </cell>
+          <cell r="T9">
+            <v>12.814590000000001</v>
+          </cell>
+          <cell r="U9">
+            <v>12818.666666666666</v>
+          </cell>
+          <cell r="V9">
+            <v>61989.9</v>
+          </cell>
+          <cell r="X9">
+            <v>221159.28125666664</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>FTTB_UDWDM_100</v>
+          </cell>
+          <cell r="S10">
+            <v>78872.09</v>
+          </cell>
+          <cell r="T10">
+            <v>14.612120000000001</v>
+          </cell>
+          <cell r="U10">
+            <v>5866.833333333333</v>
+          </cell>
+          <cell r="V10">
+            <v>63060</v>
+          </cell>
+          <cell r="X10">
+            <v>147813.53545333334</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>FTTC_Hybridpon_25</v>
+          </cell>
+          <cell r="S11">
+            <v>114876.4</v>
+          </cell>
+          <cell r="T11">
+            <v>12.59423</v>
+          </cell>
+          <cell r="U11">
+            <v>4000</v>
+          </cell>
+          <cell r="V11">
+            <v>96145</v>
+          </cell>
+          <cell r="X11">
+            <v>215033.99423000001</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>FTTB_Hybridpon_50</v>
+          </cell>
+          <cell r="S12">
+            <v>115530.5</v>
+          </cell>
+          <cell r="T12">
+            <v>12.21167</v>
+          </cell>
+          <cell r="U12">
+            <v>7280</v>
+          </cell>
+          <cell r="V12">
+            <v>55966.5</v>
+          </cell>
+          <cell r="X12">
+            <v>178789.21166999999</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>FTTH_Hybridpon_100</v>
+          </cell>
+          <cell r="S13">
+            <v>115530.5</v>
+          </cell>
+          <cell r="T13">
+            <v>25.08727</v>
+          </cell>
+          <cell r="U13">
+            <v>14160</v>
+          </cell>
+          <cell r="V13">
+            <v>168466.5</v>
+          </cell>
+          <cell r="X13">
+            <v>298182.08727000002</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>FTTC_Hybridpon_100</v>
+          </cell>
+          <cell r="S14">
+            <v>114876.4</v>
+          </cell>
+          <cell r="T14">
+            <v>12.59423</v>
+          </cell>
+          <cell r="U14">
+            <v>14800</v>
+          </cell>
+          <cell r="V14">
+            <v>105356</v>
+          </cell>
+          <cell r="X14">
+            <v>235044.99423000001</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>FTTB_Hybridpon_100</v>
+          </cell>
+          <cell r="S15">
+            <v>115530.5</v>
+          </cell>
+          <cell r="T15">
+            <v>12.21167</v>
+          </cell>
+          <cell r="U15">
+            <v>14160</v>
+          </cell>
+          <cell r="V15">
+            <v>66966.5</v>
+          </cell>
+          <cell r="X15">
+            <v>196669.21166999999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2600,8 +3574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +3598,7 @@
     <col min="24" max="24" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2698,7 +3672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -2740,7 +3714,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -2815,11 +3789,11 @@
         <v>161610.48888888888</v>
       </c>
       <c r="X3" s="12">
-        <f t="shared" ref="X3:X14" si="0">S3+T3+U3+V3</f>
+        <f>S3+T3+U3+V3</f>
         <v>307967.22911888885</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -2889,15 +3863,15 @@
         <v>63750.8</v>
       </c>
       <c r="W4" s="11">
-        <f t="shared" ref="W4:W15" si="1">SUM(U4,V4)</f>
+        <f t="shared" ref="W4:W15" si="0">SUM(U4,V4)</f>
         <v>70156.133333333331</v>
       </c>
       <c r="X4" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="X4:X14" si="1">S4+T4+U4+V4</f>
         <v>216506.84792333335</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -2963,15 +3937,15 @@
         <v>60860</v>
       </c>
       <c r="W5" s="11">
+        <f t="shared" si="0"/>
+        <v>66159.166666666672</v>
+      </c>
+      <c r="X5" s="12">
         <f t="shared" si="1"/>
-        <v>66159.166666666672</v>
-      </c>
-      <c r="X5" s="12">
-        <f t="shared" si="0"/>
         <v>145045.86878666666</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -3041,15 +4015,15 @@
         <v>133338.59999999998</v>
       </c>
       <c r="W6" s="11">
+        <f t="shared" si="0"/>
+        <v>139205.43333333332</v>
+      </c>
+      <c r="X6" s="12">
         <f t="shared" si="1"/>
-        <v>139205.43333333332</v>
-      </c>
-      <c r="X6" s="12">
-        <f t="shared" si="0"/>
         <v>218092.13545333332</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -3119,15 +4093,15 @@
         <v>129280.20000000001</v>
       </c>
       <c r="W7" s="11">
+        <f t="shared" si="0"/>
+        <v>141898.86666666667</v>
+      </c>
+      <c r="X7" s="12">
         <f t="shared" si="1"/>
-        <v>141898.86666666667</v>
-      </c>
-      <c r="X7" s="12">
-        <f t="shared" si="0"/>
         <v>288249.58125666669</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -3195,15 +4169,15 @@
         <v>195086.4</v>
       </c>
       <c r="W8" s="11">
+        <f t="shared" si="0"/>
+        <v>201513.06666666665</v>
+      </c>
+      <c r="X8" s="12">
         <f t="shared" si="1"/>
-        <v>201513.06666666665</v>
-      </c>
-      <c r="X8" s="12">
-        <f t="shared" si="0"/>
         <v>347869.80689666665</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -3271,15 +4245,15 @@
         <v>61989.9</v>
       </c>
       <c r="W9" s="11">
+        <f t="shared" si="0"/>
+        <v>74808.566666666666</v>
+      </c>
+      <c r="X9" s="12">
         <f t="shared" si="1"/>
-        <v>74808.566666666666</v>
-      </c>
-      <c r="X9" s="12">
-        <f t="shared" si="0"/>
         <v>221159.28125666664</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -3340,21 +4314,21 @@
         <v>14.612120000000001</v>
       </c>
       <c r="U10" s="11">
-        <v>11216.333333333334</v>
+        <v>5866.833333333333</v>
       </c>
       <c r="V10" s="11">
         <v>63060</v>
       </c>
       <c r="W10" s="11">
+        <f t="shared" si="0"/>
+        <v>68926.833333333328</v>
+      </c>
+      <c r="X10" s="12">
         <f t="shared" si="1"/>
-        <v>74276.333333333328</v>
-      </c>
-      <c r="X10" s="12">
-        <f t="shared" si="0"/>
-        <v>153163.03545333334</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>147813.53545333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -3423,15 +4397,15 @@
         <v>96145</v>
       </c>
       <c r="W11" s="11">
+        <f t="shared" si="0"/>
+        <v>100145</v>
+      </c>
+      <c r="X11" s="12">
         <f t="shared" si="1"/>
-        <v>100145</v>
-      </c>
-      <c r="X11" s="12">
-        <f t="shared" si="0"/>
         <v>215033.99423000001</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -3499,15 +4473,15 @@
         <v>55966.5</v>
       </c>
       <c r="W12" s="11">
+        <f t="shared" si="0"/>
+        <v>63246.5</v>
+      </c>
+      <c r="X12" s="12">
         <f t="shared" si="1"/>
-        <v>63246.5</v>
-      </c>
-      <c r="X12" s="12">
-        <f t="shared" si="0"/>
         <v>178789.21166999999</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -3576,15 +4550,15 @@
         <v>168466.5</v>
       </c>
       <c r="W13" s="11">
+        <f t="shared" si="0"/>
+        <v>182626.5</v>
+      </c>
+      <c r="X13" s="12">
         <f t="shared" si="1"/>
-        <v>182626.5</v>
-      </c>
-      <c r="X13" s="12">
-        <f t="shared" si="0"/>
         <v>298182.08727000002</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -3646,21 +4620,21 @@
         <v>12.59423</v>
       </c>
       <c r="U14" s="11">
-        <v>27600</v>
+        <v>14800</v>
       </c>
       <c r="V14" s="11">
         <v>105356</v>
       </c>
       <c r="W14" s="11">
+        <f t="shared" si="0"/>
+        <v>120156</v>
+      </c>
+      <c r="X14" s="12">
         <f t="shared" si="1"/>
-        <v>132956</v>
-      </c>
-      <c r="X14" s="12">
-        <f t="shared" si="0"/>
-        <v>247844.99423000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>235044.99423000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -3729,7 +4703,7 @@
         <v>66966.5</v>
       </c>
       <c r="W15" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>81126.5</v>
       </c>
       <c r="X15" s="12">
@@ -3737,7 +4711,7 @@
         <v>196669.21166999999</v>
       </c>
     </row>
-    <row r="27" spans="17:17" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q27">
         <f>0.02/1000</f>
         <v>2.0000000000000002E-5</v>
@@ -15384,8 +16358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15407,7 +16381,7 @@
     <col min="15" max="15" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -15454,7 +16428,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -15462,59 +16436,59 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>CAPEX!$X3</f>
+        <f>[1]CAPEX!$X3</f>
         <v>307967.22911888885</v>
       </c>
       <c r="D2">
-        <f>CAPEX!$X4</f>
+        <f>[1]CAPEX!$X4</f>
         <v>216506.84792333335</v>
       </c>
       <c r="E2">
-        <f>CAPEX!$X5</f>
+        <f>[1]CAPEX!$X5</f>
         <v>145045.86878666666</v>
       </c>
       <c r="F2">
-        <f>CAPEX!$X6</f>
+        <f>[1]CAPEX!$X6</f>
         <v>218092.13545333332</v>
       </c>
       <c r="G2">
-        <f>CAPEX!$X7</f>
+        <f>[1]CAPEX!$X7</f>
         <v>288249.58125666669</v>
       </c>
       <c r="H2">
-        <f>CAPEX!$X8</f>
+        <f>[1]CAPEX!$X8</f>
         <v>347869.80689666665</v>
       </c>
       <c r="I2">
-        <f>CAPEX!$X9</f>
+        <f>[1]CAPEX!$X9</f>
         <v>221159.28125666664</v>
       </c>
       <c r="J2">
-        <f>CAPEX!$X10</f>
-        <v>153163.03545333334</v>
+        <f>[1]CAPEX!$X10</f>
+        <v>147813.53545333334</v>
       </c>
       <c r="K2">
-        <f>CAPEX!$X11</f>
+        <f>[1]CAPEX!$X11</f>
         <v>215033.99423000001</v>
       </c>
       <c r="L2">
-        <f>CAPEX!$X12</f>
+        <f>[1]CAPEX!$X12</f>
         <v>178789.21166999999</v>
       </c>
       <c r="M2">
-        <f>CAPEX!$X13</f>
+        <f>[1]CAPEX!$X13</f>
         <v>298182.08727000002</v>
       </c>
       <c r="N2">
-        <f>CAPEX!$X14</f>
-        <v>247844.99423000001</v>
+        <f>[1]CAPEX!$X14</f>
+        <v>235044.99423000001</v>
       </c>
       <c r="O2">
-        <f>CAPEX!$X15</f>
+        <f>[1]CAPEX!$X15</f>
         <v>196669.21166999999</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -15525,8 +16499,8 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>D2-C2</f>
-        <v>-91460.381195555499</v>
+        <f>IF(D2-C2&gt;0,D2-C2,0)</f>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -15535,8 +16509,8 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>G2-C2</f>
-        <v>-19717.647862222162</v>
+        <f>IF(G2-C2&gt;0,G2-C2,0)</f>
+        <v>0</v>
       </c>
       <c r="H3">
         <f>H2-C2</f>
@@ -15544,7 +16518,7 @@
       </c>
       <c r="I3">
         <f>I2-D2+D3</f>
-        <v>-86807.947862222209</v>
+        <v>4652.4333333332906</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -15565,7 +16539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -15614,7 +16588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -15645,7 +16619,7 @@
       </c>
       <c r="J5">
         <f>J2-E2</f>
-        <v>8117.1666666666861</v>
+        <v>2767.6666666666861</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -15663,7 +16637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -15710,7 +16684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -15757,7 +16731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -15777,15 +16751,15 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>G2-H2</f>
-        <v>-59620.225639999961</v>
+        <f>IF(G2-H2&gt;0,G2-H2,0)</f>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <f>I2-H2</f>
-        <v>-126710.52564000001</v>
+        <f>IF(I2-H2&gt;0,I2-H2,0)</f>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -15806,7 +16780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -15854,7 +16828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -15872,7 +16846,7 @@
       </c>
       <c r="F10">
         <f>F2-J2</f>
-        <v>64929.099999999977</v>
+        <v>70278.599999999977</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -15902,7 +16876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -15937,8 +16911,8 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <f>L2-K2</f>
-        <v>-36244.782560000021</v>
+        <f>IF(L2-K2&gt;0,L2-K2,0)</f>
+        <v>0</v>
       </c>
       <c r="M11">
         <f>M2-K2</f>
@@ -15946,14 +16920,14 @@
       </c>
       <c r="N11">
         <f>N2-K2</f>
-        <v>32811</v>
+        <v>20011</v>
       </c>
       <c r="O11">
         <f>O2-L2+L11</f>
-        <v>-18364.782560000021</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>17880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -16002,7 +16976,7 @@
         <v>17880</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -16049,7 +17023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -16088,17 +17062,17 @@
       </c>
       <c r="M14">
         <f>M2-N2</f>
-        <v>50337.093040000007</v>
+        <v>63137.093040000007</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <f>O2-N2</f>
-        <v>-51175.782560000021</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IF(O2-N2&gt;0,O2-N2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -16171,8 +17145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16195,8 +17169,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="12">
-        <f>AVERAGE(B3:B15)</f>
-        <v>36062.342937580564</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -16314,7 +17287,7 @@
   <dimension ref="A1:AH74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H18"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>